<commit_message>
remove blasted external linkages!
</commit_message>
<xml_diff>
--- a/EC/Train Runs and Enforcements 2016-05-26.xlsx
+++ b/EC/Train Runs and Enforcements 2016-05-26.xlsx
@@ -34,7 +34,7 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="Denver Train Runs 04122016" type="6" refreshedVersion="5" background="1" saveData="1">
+  <connection id="1" name="Denver Train Runs 04122016" type="6" refreshedVersion="5" deleted="1" background="1" saveData="1">
     <textPr codePage="437" sourceFile="C:\Users\rwhitlock\Desktop\Denver Train Runs 04122016.txt">
       <textFields count="10">
         <textField/>
@@ -2788,7 +2788,7 @@
   <dimension ref="A1:CK157"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A73" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q84" sqref="Q84"/>
+      <selection activeCell="Q83" sqref="Q83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>